<commit_message>
add constraint for equipment assignment
</commit_message>
<xml_diff>
--- a/DensoHack/ManPower/InputSample.xlsx
+++ b/DensoHack/ManPower/InputSample.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\dmo_ortools\DensoHack\ManPower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EA7088-1781-409C-9B4B-16F963B0F36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1899A6F2-5B08-421F-AE71-A849BBD7BD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{551AB8C5-5540-4732-8D93-C6C5F6AE88B8}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData" sheetId="1" r:id="rId1"/>
     <sheet name="LineStage" sheetId="2" r:id="rId2"/>
-    <sheet name="WorkerStageAllowance" sheetId="3" r:id="rId3"/>
-    <sheet name="WorkerShift" sheetId="4" r:id="rId4"/>
-    <sheet name="WorkerPreassigned" sheetId="5" r:id="rId5"/>
+    <sheet name="EquipmentFunction" sheetId="7" r:id="rId3"/>
+    <sheet name="WorkerStageAllowance" sheetId="3" r:id="rId4"/>
+    <sheet name="LineFunctionRequirement" sheetId="6" r:id="rId5"/>
+    <sheet name="WorkerShift" sheetId="4" r:id="rId6"/>
+    <sheet name="WorkerPreassigned" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="106">
   <si>
     <t>NumOfLines</t>
   </si>
@@ -47,9 +49,6 @@
   </si>
   <si>
     <t>NumOfStages</t>
-  </si>
-  <si>
-    <t>NumOfDays</t>
   </si>
   <si>
     <t>NumOfEquipments</t>
@@ -269,6 +268,96 @@
   </si>
   <si>
     <t>S29</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>E14</t>
+  </si>
+  <si>
+    <t>E15</t>
+  </si>
+  <si>
+    <t>E16</t>
+  </si>
+  <si>
+    <t>E17</t>
+  </si>
+  <si>
+    <t>E18</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>F0</t>
   </si>
 </sst>
 </file>
@@ -726,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3D0BE5-8F81-4FA6-8273-61CC5983DFE1}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,42 +828,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B1" s="4">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,15 +871,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -800,29 +881,110 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833D5601-FB4B-4B18-BE5D-E8581E793CCA}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:AE11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -833,123 +995,852 @@
       <c r="D2" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <v>1</v>
+      </c>
+      <c r="L2" s="6">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6">
+        <v>1</v>
+      </c>
+      <c r="N2" s="6">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6">
+        <v>1</v>
+      </c>
+      <c r="P2" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>1</v>
+      </c>
+      <c r="R2" s="6">
+        <v>1</v>
+      </c>
+      <c r="S2" s="6">
+        <v>1</v>
+      </c>
+      <c r="T2" s="6">
+        <v>1</v>
+      </c>
+      <c r="U2" s="6">
+        <v>1</v>
+      </c>
+      <c r="V2" s="6">
+        <v>1</v>
+      </c>
+      <c r="W2" s="6">
+        <v>1</v>
+      </c>
+      <c r="X2" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6">
+        <v>1</v>
+      </c>
+      <c r="L3" s="6">
+        <v>1</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1</v>
+      </c>
+      <c r="N3" s="6">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>1</v>
+      </c>
+      <c r="R3" s="6">
+        <v>1</v>
+      </c>
+      <c r="S3" s="6">
+        <v>1</v>
+      </c>
+      <c r="T3" s="6">
+        <v>1</v>
+      </c>
+      <c r="U3" s="6">
+        <v>1</v>
+      </c>
+      <c r="V3" s="6">
+        <v>1</v>
+      </c>
+      <c r="W3" s="6">
+        <v>1</v>
+      </c>
+      <c r="X3" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7">
+        <v>1</v>
+      </c>
+      <c r="O4" s="7">
+        <v>1</v>
+      </c>
+      <c r="P4" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>1</v>
+      </c>
+      <c r="R4" s="7">
+        <v>1</v>
+      </c>
+      <c r="S4" s="7">
+        <v>1</v>
+      </c>
+      <c r="T4" s="7">
+        <v>1</v>
+      </c>
+      <c r="U4" s="7">
+        <v>1</v>
+      </c>
+      <c r="V4" s="7">
+        <v>1</v>
+      </c>
+      <c r="W4" s="7">
+        <v>1</v>
+      </c>
+      <c r="X4" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6">
+        <v>1</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6">
+        <v>1</v>
+      </c>
+      <c r="O5" s="6">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>1</v>
+      </c>
+      <c r="R5" s="6">
+        <v>1</v>
+      </c>
+      <c r="S5" s="6">
+        <v>1</v>
+      </c>
+      <c r="T5" s="6">
+        <v>1</v>
+      </c>
+      <c r="U5" s="6">
+        <v>1</v>
+      </c>
+      <c r="V5" s="6">
+        <v>1</v>
+      </c>
+      <c r="W5" s="6">
+        <v>1</v>
+      </c>
+      <c r="X5" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="6">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
+        <v>1</v>
+      </c>
+      <c r="P6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="6">
+        <v>1</v>
+      </c>
+      <c r="S6" s="6">
+        <v>1</v>
+      </c>
+      <c r="T6" s="6">
+        <v>1</v>
+      </c>
+      <c r="U6" s="6">
+        <v>1</v>
+      </c>
+      <c r="V6" s="6">
+        <v>1</v>
+      </c>
+      <c r="W6" s="6">
+        <v>1</v>
+      </c>
+      <c r="X6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
+        <v>1</v>
+      </c>
+      <c r="L7" s="6">
+        <v>1</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
+      <c r="N7" s="6">
+        <v>1</v>
+      </c>
+      <c r="O7" s="6">
+        <v>1</v>
+      </c>
+      <c r="P7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>1</v>
+      </c>
+      <c r="R7" s="6">
+        <v>1</v>
+      </c>
+      <c r="S7" s="6">
+        <v>1</v>
+      </c>
+      <c r="T7" s="6">
+        <v>1</v>
+      </c>
+      <c r="U7" s="6">
+        <v>1</v>
+      </c>
+      <c r="V7" s="6">
+        <v>1</v>
+      </c>
+      <c r="W7" s="6">
+        <v>1</v>
+      </c>
+      <c r="X7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1</v>
+      </c>
+      <c r="L8" s="6">
+        <v>1</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1</v>
+      </c>
+      <c r="N8" s="6">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6">
+        <v>1</v>
+      </c>
+      <c r="P8" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>1</v>
+      </c>
+      <c r="R8" s="6">
+        <v>1</v>
+      </c>
+      <c r="S8" s="6">
+        <v>1</v>
+      </c>
+      <c r="T8" s="6">
+        <v>1</v>
+      </c>
+      <c r="U8" s="6">
+        <v>1</v>
+      </c>
+      <c r="V8" s="6">
+        <v>1</v>
+      </c>
+      <c r="W8" s="6">
+        <v>1</v>
+      </c>
+      <c r="X8" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1</v>
+      </c>
+      <c r="L9" s="6">
+        <v>1</v>
+      </c>
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
+      <c r="N9" s="6">
+        <v>1</v>
+      </c>
+      <c r="O9" s="6">
+        <v>1</v>
+      </c>
+      <c r="P9" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>1</v>
+      </c>
+      <c r="R9" s="6">
+        <v>1</v>
+      </c>
+      <c r="S9" s="6">
+        <v>1</v>
+      </c>
+      <c r="T9" s="6">
+        <v>1</v>
+      </c>
+      <c r="U9" s="6">
+        <v>1</v>
+      </c>
+      <c r="V9" s="6">
+        <v>1</v>
+      </c>
+      <c r="W9" s="6">
+        <v>1</v>
+      </c>
+      <c r="X9" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6">
+        <v>1</v>
+      </c>
+      <c r="L10" s="6">
+        <v>1</v>
+      </c>
+      <c r="M10" s="6">
+        <v>1</v>
+      </c>
+      <c r="N10" s="6">
+        <v>1</v>
+      </c>
+      <c r="O10" s="6">
+        <v>1</v>
+      </c>
+      <c r="P10" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>1</v>
+      </c>
+      <c r="R10" s="6">
+        <v>1</v>
+      </c>
+      <c r="S10" s="6">
+        <v>1</v>
+      </c>
+      <c r="T10" s="6">
+        <v>1</v>
+      </c>
+      <c r="U10" s="6">
+        <v>1</v>
+      </c>
+      <c r="V10" s="6">
+        <v>1</v>
+      </c>
+      <c r="W10" s="6">
+        <v>1</v>
+      </c>
+      <c r="X10" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="B11" s="6">
         <v>1</v>
       </c>
@@ -959,19 +1850,851 @@
       <c r="D11" s="6">
         <v>1</v>
       </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6">
+        <v>1</v>
+      </c>
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11" s="6">
+        <v>1</v>
+      </c>
+      <c r="O11" s="6">
+        <v>1</v>
+      </c>
+      <c r="P11" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>1</v>
+      </c>
+      <c r="R11" s="6">
+        <v>1</v>
+      </c>
+      <c r="S11" s="6">
+        <v>1</v>
+      </c>
+      <c r="T11" s="6">
+        <v>1</v>
+      </c>
+      <c r="U11" s="6">
+        <v>1</v>
+      </c>
+      <c r="V11" s="6">
+        <v>1</v>
+      </c>
+      <c r="W11" s="6">
+        <v>1</v>
+      </c>
+      <c r="X11" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB8EDC6-9709-4016-B731-A1658E46D26E}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9994A7CA-23EA-4C65-AFB2-0395BC2CA510}">
   <dimension ref="A1:AF31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,100 +2702,100 @@
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="AE1" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="AF1" s="2"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1168,7 +2891,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1264,7 +2987,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -1360,7 +3083,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -1455,7 +3178,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -1550,7 +3273,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -1645,7 +3368,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -1740,7 +3463,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -1835,7 +3558,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -1930,7 +3653,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -2025,7 +3748,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -2120,7 +3843,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -2215,7 +3938,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -2310,7 +4033,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -2405,7 +4128,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -2500,7 +4223,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -2595,7 +4318,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -2690,7 +4413,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
@@ -2785,7 +4508,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -2880,7 +4603,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
@@ -2975,7 +4698,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
@@ -3070,7 +4793,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
@@ -3165,7 +4888,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
@@ -3260,7 +4983,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
@@ -3355,7 +5078,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
@@ -3450,7 +5173,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
@@ -3545,7 +5268,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
@@ -3640,7 +5363,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -3735,7 +5458,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
@@ -3830,7 +5553,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
@@ -3929,12 +5652,469 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8310249D-D1B0-4258-B075-6C99C40C60C4}">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728D9C57-200C-4D92-8B83-A034DA133908}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3942,64 +6122,64 @@
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>50</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
@@ -4014,7 +6194,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -4089,7 +6269,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -4164,7 +6344,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -4239,7 +6419,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -4304,7 +6484,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -4369,7 +6549,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -4434,7 +6614,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -4499,7 +6679,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -4564,7 +6744,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -4629,7 +6809,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -4694,7 +6874,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -4759,7 +6939,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -4824,7 +7004,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -4889,7 +7069,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -4954,7 +7134,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -5019,7 +7199,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -5084,7 +7264,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -5149,7 +7329,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
@@ -5214,7 +7394,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -5279,7 +7459,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
@@ -5344,7 +7524,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
@@ -5409,7 +7589,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
@@ -5474,7 +7654,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
@@ -5539,7 +7719,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
@@ -5604,7 +7784,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
@@ -5669,7 +7849,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
@@ -5734,7 +7914,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
@@ -5799,7 +7979,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -5864,7 +8044,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
@@ -5929,7 +8109,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
@@ -5998,12 +8178,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63DA2F9-D242-4008-BE35-DE7F159F8A91}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6011,99 +8191,99 @@
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="AE1" s="8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -6198,7 +8378,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -6293,7 +8473,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -6388,7 +8568,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -6483,7 +8663,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -6578,7 +8758,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -6673,7 +8853,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -6768,7 +8948,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -6863,7 +9043,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -6958,7 +9138,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -7053,7 +9233,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -7148,7 +9328,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -7243,7 +9423,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -7338,7 +9518,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -7433,7 +9613,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -7528,7 +9708,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -7623,7 +9803,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="3">
         <v>0</v>
@@ -7718,7 +9898,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -7813,7 +9993,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -7908,7 +10088,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -8003,7 +10183,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -8098,7 +10278,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -8193,7 +10373,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
@@ -8288,7 +10468,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
@@ -8383,7 +10563,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="3">
         <v>0</v>
@@ -8478,7 +10658,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
@@ -8573,7 +10753,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -8668,7 +10848,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
@@ -8763,7 +10943,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
@@ -8858,7 +11038,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
add Calculate Productivity func
</commit_message>
<xml_diff>
--- a/DensoHack/ManPower/InputSample.xlsx
+++ b/DensoHack/ManPower/InputSample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\dmo_ortools\DensoHack\ManPower\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trung\Documents\GitHub\dmo_ortools\DensoHack\ManPower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1899A6F2-5B08-421F-AE71-A849BBD7BD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694FEE9D-8EB8-437A-BF40-BF0DE04E6344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{551AB8C5-5540-4732-8D93-C6C5F6AE88B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="9" xr2:uid="{551AB8C5-5540-4732-8D93-C6C5F6AE88B8}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="LineFunctionRequirement" sheetId="6" r:id="rId5"/>
     <sheet name="WorkerShift" sheetId="4" r:id="rId6"/>
     <sheet name="WorkerPreassigned" sheetId="5" r:id="rId7"/>
+    <sheet name="EquipmentProductivityScore" sheetId="8" r:id="rId8"/>
+    <sheet name="WorkerStageExperience" sheetId="9" r:id="rId9"/>
+    <sheet name="WorkerProfile" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="110">
   <si>
     <t>NumOfLines</t>
   </si>
@@ -359,6 +362,18 @@
   <si>
     <t>F0</t>
   </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
 </sst>
 </file>
 
@@ -473,7 +488,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -498,6 +513,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -818,7 +836,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,6 +890,453 @@
       </c>
       <c r="B6" s="4">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462ECC44-A375-48A7-B11B-1E62D1C8EECF}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3">
+        <v>21</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3">
+        <v>21</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="3">
+        <v>21</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="3">
+        <v>21</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="3">
+        <v>21</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3">
+        <v>21</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="3">
+        <v>21</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="3">
+        <v>21</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="3">
+        <v>21</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="3">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="3">
+        <v>21</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1944,7 +2409,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+      <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,8 +3158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9994A7CA-23EA-4C65-AFB2-0395BC2CA510}">
   <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A31"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5656,8 +6121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8310249D-D1B0-4258-B075-6C99C40C60C4}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11134,4 +11599,3143 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122F9169-46BA-42B9-B652-34E228F53F00}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="4">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8C6B3D-87E7-4B8A-AD50-76DEB59FF5C4}">
+  <dimension ref="A1:AE31"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:AE1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3">
+        <v>1</v>
+      </c>
+      <c r="P2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
+        <v>1</v>
+      </c>
+      <c r="S2" s="3">
+        <v>1</v>
+      </c>
+      <c r="T2" s="3">
+        <v>1</v>
+      </c>
+      <c r="U2" s="3">
+        <v>1</v>
+      </c>
+      <c r="V2" s="3">
+        <v>1</v>
+      </c>
+      <c r="W2" s="3">
+        <v>1</v>
+      </c>
+      <c r="X2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <v>1</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3">
+        <v>1</v>
+      </c>
+      <c r="S3" s="3">
+        <v>1</v>
+      </c>
+      <c r="T3" s="3">
+        <v>1</v>
+      </c>
+      <c r="U3" s="3">
+        <v>1</v>
+      </c>
+      <c r="V3" s="3">
+        <v>1</v>
+      </c>
+      <c r="W3" s="3">
+        <v>1</v>
+      </c>
+      <c r="X3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1</v>
+      </c>
+      <c r="R4" s="3">
+        <v>1</v>
+      </c>
+      <c r="S4" s="3">
+        <v>1</v>
+      </c>
+      <c r="T4" s="3">
+        <v>1</v>
+      </c>
+      <c r="U4" s="3">
+        <v>1</v>
+      </c>
+      <c r="V4" s="3">
+        <v>1</v>
+      </c>
+      <c r="W4" s="3">
+        <v>1</v>
+      </c>
+      <c r="X4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3">
+        <v>1</v>
+      </c>
+      <c r="S5" s="3">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3">
+        <v>1</v>
+      </c>
+      <c r="U5" s="3">
+        <v>1</v>
+      </c>
+      <c r="V5" s="3">
+        <v>1</v>
+      </c>
+      <c r="W5" s="3">
+        <v>1</v>
+      </c>
+      <c r="X5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
+        <v>1</v>
+      </c>
+      <c r="P6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3">
+        <v>1</v>
+      </c>
+      <c r="S6" s="3">
+        <v>1</v>
+      </c>
+      <c r="T6" s="3">
+        <v>1</v>
+      </c>
+      <c r="U6" s="3">
+        <v>1</v>
+      </c>
+      <c r="V6" s="3">
+        <v>1</v>
+      </c>
+      <c r="W6" s="3">
+        <v>1</v>
+      </c>
+      <c r="X6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1</v>
+      </c>
+      <c r="O7" s="3">
+        <v>1</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1</v>
+      </c>
+      <c r="R7" s="3">
+        <v>1</v>
+      </c>
+      <c r="S7" s="3">
+        <v>1</v>
+      </c>
+      <c r="T7" s="3">
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
+        <v>1</v>
+      </c>
+      <c r="V7" s="3">
+        <v>1</v>
+      </c>
+      <c r="W7" s="3">
+        <v>1</v>
+      </c>
+      <c r="X7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1</v>
+      </c>
+      <c r="O8" s="3">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1</v>
+      </c>
+      <c r="R8" s="3">
+        <v>1</v>
+      </c>
+      <c r="S8" s="3">
+        <v>1</v>
+      </c>
+      <c r="T8" s="3">
+        <v>1</v>
+      </c>
+      <c r="U8" s="3">
+        <v>1</v>
+      </c>
+      <c r="V8" s="3">
+        <v>1</v>
+      </c>
+      <c r="W8" s="3">
+        <v>1</v>
+      </c>
+      <c r="X8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
+      <c r="R9" s="3">
+        <v>1</v>
+      </c>
+      <c r="S9" s="3">
+        <v>1</v>
+      </c>
+      <c r="T9" s="3">
+        <v>1</v>
+      </c>
+      <c r="U9" s="3">
+        <v>1</v>
+      </c>
+      <c r="V9" s="3">
+        <v>1</v>
+      </c>
+      <c r="W9" s="3">
+        <v>1</v>
+      </c>
+      <c r="X9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1</v>
+      </c>
+      <c r="O10" s="3">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1</v>
+      </c>
+      <c r="R10" s="3">
+        <v>1</v>
+      </c>
+      <c r="S10" s="3">
+        <v>1</v>
+      </c>
+      <c r="T10" s="3">
+        <v>1</v>
+      </c>
+      <c r="U10" s="3">
+        <v>1</v>
+      </c>
+      <c r="V10" s="3">
+        <v>1</v>
+      </c>
+      <c r="W10" s="3">
+        <v>1</v>
+      </c>
+      <c r="X10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3">
+        <v>1</v>
+      </c>
+      <c r="P11" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>1</v>
+      </c>
+      <c r="R11" s="3">
+        <v>1</v>
+      </c>
+      <c r="S11" s="3">
+        <v>1</v>
+      </c>
+      <c r="T11" s="3">
+        <v>1</v>
+      </c>
+      <c r="U11" s="3">
+        <v>1</v>
+      </c>
+      <c r="V11" s="3">
+        <v>1</v>
+      </c>
+      <c r="W11" s="3">
+        <v>1</v>
+      </c>
+      <c r="X11" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>1</v>
+      </c>
+      <c r="R12" s="3">
+        <v>1</v>
+      </c>
+      <c r="S12" s="3">
+        <v>1</v>
+      </c>
+      <c r="T12" s="3">
+        <v>1</v>
+      </c>
+      <c r="U12" s="3">
+        <v>1</v>
+      </c>
+      <c r="V12" s="3">
+        <v>1</v>
+      </c>
+      <c r="W12" s="3">
+        <v>1</v>
+      </c>
+      <c r="X12" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3">
+        <v>1</v>
+      </c>
+      <c r="P13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>1</v>
+      </c>
+      <c r="R13" s="3">
+        <v>1</v>
+      </c>
+      <c r="S13" s="3">
+        <v>1</v>
+      </c>
+      <c r="T13" s="3">
+        <v>1</v>
+      </c>
+      <c r="U13" s="3">
+        <v>1</v>
+      </c>
+      <c r="V13" s="3">
+        <v>1</v>
+      </c>
+      <c r="W13" s="3">
+        <v>1</v>
+      </c>
+      <c r="X13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1</v>
+      </c>
+      <c r="N14" s="3">
+        <v>1</v>
+      </c>
+      <c r="O14" s="3">
+        <v>1</v>
+      </c>
+      <c r="P14" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>1</v>
+      </c>
+      <c r="R14" s="3">
+        <v>1</v>
+      </c>
+      <c r="S14" s="3">
+        <v>1</v>
+      </c>
+      <c r="T14" s="3">
+        <v>1</v>
+      </c>
+      <c r="U14" s="3">
+        <v>1</v>
+      </c>
+      <c r="V14" s="3">
+        <v>1</v>
+      </c>
+      <c r="W14" s="3">
+        <v>1</v>
+      </c>
+      <c r="X14" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3">
+        <v>1</v>
+      </c>
+      <c r="P15" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1</v>
+      </c>
+      <c r="R15" s="3">
+        <v>1</v>
+      </c>
+      <c r="S15" s="3">
+        <v>1</v>
+      </c>
+      <c r="T15" s="3">
+        <v>1</v>
+      </c>
+      <c r="U15" s="3">
+        <v>1</v>
+      </c>
+      <c r="V15" s="3">
+        <v>1</v>
+      </c>
+      <c r="W15" s="3">
+        <v>1</v>
+      </c>
+      <c r="X15" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1</v>
+      </c>
+      <c r="N16" s="3">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3">
+        <v>1</v>
+      </c>
+      <c r="P16" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>1</v>
+      </c>
+      <c r="R16" s="3">
+        <v>1</v>
+      </c>
+      <c r="S16" s="3">
+        <v>1</v>
+      </c>
+      <c r="T16" s="3">
+        <v>1</v>
+      </c>
+      <c r="U16" s="3">
+        <v>1</v>
+      </c>
+      <c r="V16" s="3">
+        <v>1</v>
+      </c>
+      <c r="W16" s="3">
+        <v>1</v>
+      </c>
+      <c r="X16" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3">
+        <v>1</v>
+      </c>
+      <c r="N17" s="3">
+        <v>1</v>
+      </c>
+      <c r="O17" s="3">
+        <v>1</v>
+      </c>
+      <c r="P17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1</v>
+      </c>
+      <c r="R17" s="3">
+        <v>1</v>
+      </c>
+      <c r="S17" s="3">
+        <v>1</v>
+      </c>
+      <c r="T17" s="3">
+        <v>1</v>
+      </c>
+      <c r="U17" s="3">
+        <v>1</v>
+      </c>
+      <c r="V17" s="3">
+        <v>1</v>
+      </c>
+      <c r="W17" s="3">
+        <v>1</v>
+      </c>
+      <c r="X17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3">
+        <v>1</v>
+      </c>
+      <c r="O18" s="3">
+        <v>1</v>
+      </c>
+      <c r="P18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3">
+        <v>1</v>
+      </c>
+      <c r="S18" s="3">
+        <v>1</v>
+      </c>
+      <c r="T18" s="3">
+        <v>1</v>
+      </c>
+      <c r="U18" s="3">
+        <v>1</v>
+      </c>
+      <c r="V18" s="3">
+        <v>1</v>
+      </c>
+      <c r="W18" s="3">
+        <v>1</v>
+      </c>
+      <c r="X18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1</v>
+      </c>
+      <c r="M19" s="3">
+        <v>1</v>
+      </c>
+      <c r="N19" s="3">
+        <v>1</v>
+      </c>
+      <c r="O19" s="3">
+        <v>1</v>
+      </c>
+      <c r="P19" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>1</v>
+      </c>
+      <c r="R19" s="3">
+        <v>1</v>
+      </c>
+      <c r="S19" s="3">
+        <v>1</v>
+      </c>
+      <c r="T19" s="3">
+        <v>1</v>
+      </c>
+      <c r="U19" s="3">
+        <v>1</v>
+      </c>
+      <c r="V19" s="3">
+        <v>1</v>
+      </c>
+      <c r="W19" s="3">
+        <v>1</v>
+      </c>
+      <c r="X19" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
+      <c r="N20" s="3">
+        <v>1</v>
+      </c>
+      <c r="O20" s="3">
+        <v>1</v>
+      </c>
+      <c r="P20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>1</v>
+      </c>
+      <c r="R20" s="3">
+        <v>1</v>
+      </c>
+      <c r="S20" s="3">
+        <v>1</v>
+      </c>
+      <c r="T20" s="3">
+        <v>1</v>
+      </c>
+      <c r="U20" s="3">
+        <v>1</v>
+      </c>
+      <c r="V20" s="3">
+        <v>1</v>
+      </c>
+      <c r="W20" s="3">
+        <v>1</v>
+      </c>
+      <c r="X20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+      <c r="L21" s="3">
+        <v>1</v>
+      </c>
+      <c r="M21" s="3">
+        <v>1</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1</v>
+      </c>
+      <c r="O21" s="3">
+        <v>1</v>
+      </c>
+      <c r="P21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>1</v>
+      </c>
+      <c r="R21" s="3">
+        <v>1</v>
+      </c>
+      <c r="S21" s="3">
+        <v>1</v>
+      </c>
+      <c r="T21" s="3">
+        <v>1</v>
+      </c>
+      <c r="U21" s="3">
+        <v>1</v>
+      </c>
+      <c r="V21" s="3">
+        <v>1</v>
+      </c>
+      <c r="W21" s="3">
+        <v>1</v>
+      </c>
+      <c r="X21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3">
+        <v>1</v>
+      </c>
+      <c r="L22" s="3">
+        <v>1</v>
+      </c>
+      <c r="M22" s="3">
+        <v>1</v>
+      </c>
+      <c r="N22" s="3">
+        <v>1</v>
+      </c>
+      <c r="O22" s="3">
+        <v>1</v>
+      </c>
+      <c r="P22" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>1</v>
+      </c>
+      <c r="R22" s="3">
+        <v>1</v>
+      </c>
+      <c r="S22" s="3">
+        <v>1</v>
+      </c>
+      <c r="T22" s="3">
+        <v>1</v>
+      </c>
+      <c r="U22" s="3">
+        <v>1</v>
+      </c>
+      <c r="V22" s="3">
+        <v>1</v>
+      </c>
+      <c r="W22" s="3">
+        <v>1</v>
+      </c>
+      <c r="X22" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3">
+        <v>1</v>
+      </c>
+      <c r="L23" s="3">
+        <v>1</v>
+      </c>
+      <c r="M23" s="3">
+        <v>1</v>
+      </c>
+      <c r="N23" s="3">
+        <v>1</v>
+      </c>
+      <c r="O23" s="3">
+        <v>1</v>
+      </c>
+      <c r="P23" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>1</v>
+      </c>
+      <c r="R23" s="3">
+        <v>1</v>
+      </c>
+      <c r="S23" s="3">
+        <v>1</v>
+      </c>
+      <c r="T23" s="3">
+        <v>1</v>
+      </c>
+      <c r="U23" s="3">
+        <v>1</v>
+      </c>
+      <c r="V23" s="3">
+        <v>1</v>
+      </c>
+      <c r="W23" s="3">
+        <v>1</v>
+      </c>
+      <c r="X23" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
+        <v>1</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1</v>
+      </c>
+      <c r="K24" s="3">
+        <v>1</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1</v>
+      </c>
+      <c r="M24" s="3">
+        <v>1</v>
+      </c>
+      <c r="N24" s="3">
+        <v>1</v>
+      </c>
+      <c r="O24" s="3">
+        <v>1</v>
+      </c>
+      <c r="P24" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>1</v>
+      </c>
+      <c r="R24" s="3">
+        <v>1</v>
+      </c>
+      <c r="S24" s="3">
+        <v>1</v>
+      </c>
+      <c r="T24" s="3">
+        <v>1</v>
+      </c>
+      <c r="U24" s="3">
+        <v>1</v>
+      </c>
+      <c r="V24" s="3">
+        <v>1</v>
+      </c>
+      <c r="W24" s="3">
+        <v>1</v>
+      </c>
+      <c r="X24" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3">
+        <v>1</v>
+      </c>
+      <c r="K25" s="3">
+        <v>1</v>
+      </c>
+      <c r="L25" s="3">
+        <v>1</v>
+      </c>
+      <c r="M25" s="3">
+        <v>1</v>
+      </c>
+      <c r="N25" s="3">
+        <v>1</v>
+      </c>
+      <c r="O25" s="3">
+        <v>1</v>
+      </c>
+      <c r="P25" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>1</v>
+      </c>
+      <c r="R25" s="3">
+        <v>1</v>
+      </c>
+      <c r="S25" s="3">
+        <v>1</v>
+      </c>
+      <c r="T25" s="3">
+        <v>1</v>
+      </c>
+      <c r="U25" s="3">
+        <v>1</v>
+      </c>
+      <c r="V25" s="3">
+        <v>1</v>
+      </c>
+      <c r="W25" s="3">
+        <v>1</v>
+      </c>
+      <c r="X25" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3">
+        <v>1</v>
+      </c>
+      <c r="L26" s="3">
+        <v>1</v>
+      </c>
+      <c r="M26" s="3">
+        <v>1</v>
+      </c>
+      <c r="N26" s="3">
+        <v>1</v>
+      </c>
+      <c r="O26" s="3">
+        <v>1</v>
+      </c>
+      <c r="P26" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>1</v>
+      </c>
+      <c r="R26" s="3">
+        <v>1</v>
+      </c>
+      <c r="S26" s="3">
+        <v>1</v>
+      </c>
+      <c r="T26" s="3">
+        <v>1</v>
+      </c>
+      <c r="U26" s="3">
+        <v>1</v>
+      </c>
+      <c r="V26" s="3">
+        <v>1</v>
+      </c>
+      <c r="W26" s="3">
+        <v>1</v>
+      </c>
+      <c r="X26" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1</v>
+      </c>
+      <c r="M27" s="3">
+        <v>1</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1</v>
+      </c>
+      <c r="O27" s="3">
+        <v>1</v>
+      </c>
+      <c r="P27" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>1</v>
+      </c>
+      <c r="R27" s="3">
+        <v>1</v>
+      </c>
+      <c r="S27" s="3">
+        <v>1</v>
+      </c>
+      <c r="T27" s="3">
+        <v>1</v>
+      </c>
+      <c r="U27" s="3">
+        <v>1</v>
+      </c>
+      <c r="V27" s="3">
+        <v>1</v>
+      </c>
+      <c r="W27" s="3">
+        <v>1</v>
+      </c>
+      <c r="X27" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1</v>
+      </c>
+      <c r="K28" s="3">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3">
+        <v>1</v>
+      </c>
+      <c r="M28" s="3">
+        <v>1</v>
+      </c>
+      <c r="N28" s="3">
+        <v>1</v>
+      </c>
+      <c r="O28" s="3">
+        <v>1</v>
+      </c>
+      <c r="P28" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>1</v>
+      </c>
+      <c r="R28" s="3">
+        <v>1</v>
+      </c>
+      <c r="S28" s="3">
+        <v>1</v>
+      </c>
+      <c r="T28" s="3">
+        <v>1</v>
+      </c>
+      <c r="U28" s="3">
+        <v>1</v>
+      </c>
+      <c r="V28" s="3">
+        <v>1</v>
+      </c>
+      <c r="W28" s="3">
+        <v>1</v>
+      </c>
+      <c r="X28" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1</v>
+      </c>
+      <c r="L29" s="3">
+        <v>1</v>
+      </c>
+      <c r="M29" s="3">
+        <v>1</v>
+      </c>
+      <c r="N29" s="3">
+        <v>1</v>
+      </c>
+      <c r="O29" s="3">
+        <v>1</v>
+      </c>
+      <c r="P29" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>1</v>
+      </c>
+      <c r="R29" s="3">
+        <v>1</v>
+      </c>
+      <c r="S29" s="3">
+        <v>1</v>
+      </c>
+      <c r="T29" s="3">
+        <v>1</v>
+      </c>
+      <c r="U29" s="3">
+        <v>1</v>
+      </c>
+      <c r="V29" s="3">
+        <v>1</v>
+      </c>
+      <c r="W29" s="3">
+        <v>1</v>
+      </c>
+      <c r="X29" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1</v>
+      </c>
+      <c r="J30" s="3">
+        <v>1</v>
+      </c>
+      <c r="K30" s="3">
+        <v>1</v>
+      </c>
+      <c r="L30" s="3">
+        <v>1</v>
+      </c>
+      <c r="M30" s="3">
+        <v>1</v>
+      </c>
+      <c r="N30" s="3">
+        <v>1</v>
+      </c>
+      <c r="O30" s="3">
+        <v>1</v>
+      </c>
+      <c r="P30" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>1</v>
+      </c>
+      <c r="R30" s="3">
+        <v>1</v>
+      </c>
+      <c r="S30" s="3">
+        <v>1</v>
+      </c>
+      <c r="T30" s="3">
+        <v>1</v>
+      </c>
+      <c r="U30" s="3">
+        <v>1</v>
+      </c>
+      <c r="V30" s="3">
+        <v>1</v>
+      </c>
+      <c r="W30" s="3">
+        <v>1</v>
+      </c>
+      <c r="X30" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3">
+        <v>1</v>
+      </c>
+      <c r="L31" s="3">
+        <v>1</v>
+      </c>
+      <c r="M31" s="3">
+        <v>1</v>
+      </c>
+      <c r="N31" s="3">
+        <v>1</v>
+      </c>
+      <c r="O31" s="3">
+        <v>1</v>
+      </c>
+      <c r="P31" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>1</v>
+      </c>
+      <c r="R31" s="3">
+        <v>1</v>
+      </c>
+      <c r="S31" s="3">
+        <v>1</v>
+      </c>
+      <c r="T31" s="3">
+        <v>1</v>
+      </c>
+      <c r="U31" s="3">
+        <v>1</v>
+      </c>
+      <c r="V31" s="3">
+        <v>1</v>
+      </c>
+      <c r="W31" s="3">
+        <v>1</v>
+      </c>
+      <c r="X31" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>